<commit_message>
checking in all of the docked structures
</commit_message>
<xml_diff>
--- a/mutants/abl-mutants-trimmed.xlsx
+++ b/mutants/abl-mutants-trimmed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="-20" windowWidth="51200" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="27180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="97">
   <si>
     <t>G250R</t>
   </si>
@@ -126,9 +126,6 @@
     <t>T315A</t>
   </si>
   <si>
-    <t>V298F</t>
-  </si>
-  <si>
     <t>A399T</t>
   </si>
   <si>
@@ -307,6 +304,12 @@
   </si>
   <si>
     <t xml:space="preserve">M351T </t>
+  </si>
+  <si>
+    <t>T315N</t>
+  </si>
+  <si>
+    <t>L298F</t>
   </si>
 </sst>
 </file>
@@ -363,8 +366,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -379,11 +386,15 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -716,7 +727,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -730,7 +741,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="2"/>
     </row>
@@ -739,7 +750,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -748,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -757,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -766,7 +777,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -775,7 +786,7 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -784,7 +795,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -793,7 +804,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28">
@@ -801,7 +812,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28">
@@ -809,7 +820,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28">
@@ -817,7 +828,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28">
@@ -825,7 +836,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28">
@@ -833,7 +844,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28">
@@ -841,7 +852,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28">
@@ -849,15 +860,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28">
       <c r="A16" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28">
@@ -865,7 +876,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="28">
@@ -873,7 +884,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="28">
@@ -881,7 +892,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28">
@@ -889,7 +900,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="28">
@@ -897,7 +908,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="28">
@@ -905,7 +916,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="28">
@@ -913,7 +924,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="28">
@@ -921,15 +932,15 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="28">
       <c r="A25" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="28">
@@ -950,7 +961,7 @@
     </row>
     <row r="28" spans="1:2" ht="28">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
@@ -1022,7 +1033,7 @@
     </row>
     <row r="37" spans="1:2" ht="28">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s">
         <v>24</v>
@@ -1030,7 +1041,7 @@
     </row>
     <row r="38" spans="1:2" ht="28">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
@@ -1038,7 +1049,7 @@
     </row>
     <row r="39" spans="1:2" ht="28">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
         <v>24</v>
@@ -1046,7 +1057,7 @@
     </row>
     <row r="40" spans="1:2" ht="28">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
         <v>24</v>
@@ -1054,7 +1065,7 @@
     </row>
     <row r="41" spans="1:2" ht="28">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
         <v>24</v>
@@ -1062,7 +1073,7 @@
     </row>
     <row r="42" spans="1:2" ht="28">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
         <v>24</v>
@@ -1070,7 +1081,7 @@
     </row>
     <row r="43" spans="1:2" ht="28">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
         <v>24</v>
@@ -1078,7 +1089,7 @@
     </row>
     <row r="44" spans="1:2" ht="28">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
         <v>24</v>
@@ -1086,7 +1097,7 @@
     </row>
     <row r="45" spans="1:2" ht="28">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
         <v>24</v>
@@ -1094,7 +1105,7 @@
     </row>
     <row r="46" spans="1:2" ht="28">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
         <v>24</v>
@@ -1102,7 +1113,7 @@
     </row>
     <row r="47" spans="1:2" ht="28">
       <c r="A47" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
         <v>24</v>
@@ -1110,7 +1121,7 @@
     </row>
     <row r="48" spans="1:2" ht="28">
       <c r="A48" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
         <v>24</v>
@@ -1118,7 +1129,7 @@
     </row>
     <row r="49" spans="1:2" ht="28">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
         <v>24</v>
@@ -1126,7 +1137,7 @@
     </row>
     <row r="50" spans="1:2" ht="28">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
         <v>24</v>
@@ -1134,7 +1145,7 @@
     </row>
     <row r="51" spans="1:2" ht="28">
       <c r="A51" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
         <v>24</v>
@@ -1142,7 +1153,7 @@
     </row>
     <row r="52" spans="1:2" ht="28">
       <c r="A52" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
         <v>24</v>
@@ -1150,7 +1161,7 @@
     </row>
     <row r="53" spans="1:2" ht="28">
       <c r="A53" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
         <v>24</v>
@@ -1158,7 +1169,7 @@
     </row>
     <row r="54" spans="1:2" ht="28">
       <c r="A54" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
         <v>24</v>
@@ -1166,7 +1177,7 @@
     </row>
     <row r="55" spans="1:2" ht="28">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
         <v>24</v>
@@ -1174,7 +1185,7 @@
     </row>
     <row r="56" spans="1:2" ht="28">
       <c r="A56" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
         <v>24</v>
@@ -1182,7 +1193,7 @@
     </row>
     <row r="57" spans="1:2" ht="28">
       <c r="A57" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
         <v>24</v>
@@ -1190,7 +1201,7 @@
     </row>
     <row r="58" spans="1:2" ht="28">
       <c r="A58" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
         <v>24</v>
@@ -1198,7 +1209,7 @@
     </row>
     <row r="59" spans="1:2" ht="28">
       <c r="A59" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
         <v>24</v>
@@ -1206,7 +1217,7 @@
     </row>
     <row r="60" spans="1:2" ht="28">
       <c r="A60" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
         <v>24</v>
@@ -1214,7 +1225,7 @@
     </row>
     <row r="61" spans="1:2" ht="28">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
         <v>24</v>
@@ -1222,7 +1233,7 @@
     </row>
     <row r="62" spans="1:2" ht="28">
       <c r="A62" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
         <v>24</v>
@@ -1230,7 +1241,7 @@
     </row>
     <row r="63" spans="1:2" ht="28">
       <c r="A63" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
         <v>24</v>
@@ -1238,7 +1249,7 @@
     </row>
     <row r="64" spans="1:2" ht="28">
       <c r="A64" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
         <v>24</v>
@@ -1246,7 +1257,7 @@
     </row>
     <row r="65" spans="1:2" ht="28">
       <c r="A65" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
         <v>24</v>
@@ -1254,7 +1265,7 @@
     </row>
     <row r="66" spans="1:2" ht="28">
       <c r="A66" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" t="s">
         <v>24</v>
@@ -1262,7 +1273,7 @@
     </row>
     <row r="67" spans="1:2" ht="28">
       <c r="A67" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
         <v>24</v>
@@ -1270,7 +1281,7 @@
     </row>
     <row r="68" spans="1:2" ht="28">
       <c r="A68" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" t="s">
         <v>24</v>
@@ -1278,7 +1289,7 @@
     </row>
     <row r="69" spans="1:2" ht="28">
       <c r="A69" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" t="s">
         <v>24</v>
@@ -1286,7 +1297,7 @@
     </row>
     <row r="70" spans="1:2" ht="28">
       <c r="A70" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
         <v>24</v>
@@ -1294,7 +1305,7 @@
     </row>
     <row r="71" spans="1:2" ht="28">
       <c r="A71" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
         <v>24</v>
@@ -1302,7 +1313,7 @@
     </row>
     <row r="72" spans="1:2" ht="28">
       <c r="A72" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" t="s">
         <v>24</v>
@@ -1310,7 +1321,7 @@
     </row>
     <row r="73" spans="1:2" ht="28">
       <c r="A73" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" t="s">
         <v>24</v>
@@ -1318,7 +1329,7 @@
     </row>
     <row r="74" spans="1:2" ht="28">
       <c r="A74" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" t="s">
         <v>24</v>
@@ -1326,7 +1337,7 @@
     </row>
     <row r="75" spans="1:2" ht="28">
       <c r="A75" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" t="s">
         <v>24</v>
@@ -1334,7 +1345,7 @@
     </row>
     <row r="76" spans="1:2" ht="28">
       <c r="A76" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" t="s">
         <v>24</v>
@@ -1342,7 +1353,7 @@
     </row>
     <row r="77" spans="1:2" ht="28">
       <c r="A77" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" t="s">
         <v>24</v>
@@ -1350,7 +1361,7 @@
     </row>
     <row r="78" spans="1:2" ht="28">
       <c r="A78" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" t="s">
         <v>24</v>
@@ -1358,7 +1369,7 @@
     </row>
     <row r="79" spans="1:2" ht="28">
       <c r="A79" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" t="s">
         <v>24</v>
@@ -1366,7 +1377,7 @@
     </row>
     <row r="80" spans="1:2" ht="28">
       <c r="A80" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" t="s">
         <v>24</v>
@@ -1374,7 +1385,7 @@
     </row>
     <row r="81" spans="1:2" ht="28">
       <c r="A81" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
         <v>24</v>
@@ -1382,7 +1393,7 @@
     </row>
     <row r="82" spans="1:2" ht="28">
       <c r="A82" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" t="s">
         <v>24</v>
@@ -1390,7 +1401,7 @@
     </row>
     <row r="83" spans="1:2" ht="28">
       <c r="A83" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" t="s">
         <v>24</v>
@@ -1398,7 +1409,7 @@
     </row>
     <row r="84" spans="1:2" ht="28">
       <c r="A84" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
         <v>24</v>
@@ -1406,7 +1417,7 @@
     </row>
     <row r="85" spans="1:2" ht="28">
       <c r="A85" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" t="s">
         <v>24</v>
@@ -1414,7 +1425,7 @@
     </row>
     <row r="86" spans="1:2" ht="28">
       <c r="A86" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" t="s">
         <v>24</v>
@@ -1422,7 +1433,7 @@
     </row>
     <row r="87" spans="1:2" ht="28">
       <c r="A87" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" t="s">
         <v>24</v>
@@ -1430,7 +1441,7 @@
     </row>
     <row r="88" spans="1:2" ht="28">
       <c r="A88" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" t="s">
         <v>24</v>
@@ -1438,7 +1449,7 @@
     </row>
     <row r="89" spans="1:2" ht="28">
       <c r="A89" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
         <v>24</v>
@@ -1446,7 +1457,7 @@
     </row>
     <row r="90" spans="1:2" ht="28">
       <c r="A90" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
         <v>24</v>
@@ -1454,7 +1465,7 @@
     </row>
     <row r="91" spans="1:2" ht="28">
       <c r="A91" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
         <v>24</v>
@@ -1465,20 +1476,20 @@
         <v>0</v>
       </c>
       <c r="B92" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="28">
       <c r="A93" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="28">
       <c r="A94" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B94" t="s">
         <v>24</v>

</xml_diff>